<commit_message>
Prepared for testing Add Skill feature
</commit_message>
<xml_diff>
--- a/AutomationTesting/target/classes/dataset.xlsx
+++ b/AutomationTesting/target/classes/dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t xml:space="preserve">Testcase ID</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t xml:space="preserve">Disaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_LEAVE_TYPE_TC010</t>
   </si>
 </sst>
 </file>
@@ -196,7 +199,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -394,7 +397,7 @@
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>22</v>

</xml_diff>